<commit_message>
changed the name in dayal
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Lasith sir\Alumni_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Lasith sir\Alumni Locator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99ABEF8-6602-4DF2-B1F1-F0F72CA77319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311C5599-1FF6-44B9-8675-2F42A5314A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,9 +294,6 @@
     <t>immgs/Thanushi.jpg</t>
   </si>
   <si>
-    <t>immgs/Dayal.jpg</t>
-  </si>
-  <si>
     <t>immgs/Tharindu.jpg</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>immgs/acowshan.jpg</t>
+  </si>
+  <si>
+    <t>immgs/dayal.jpg</t>
   </si>
 </sst>
 </file>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -885,7 +885,7 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -939,7 +939,7 @@
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -956,10 +956,10 @@
         <v>2.2136999999999998</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -976,10 +976,10 @@
         <v>3.7837000000000001</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -996,10 +996,10 @@
         <v>80.751800000000003</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1016,7 +1016,7 @@
         <v>80.771799999999999</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1033,7 +1033,7 @@
         <v>80.771799999999999</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1050,7 +1050,7 @@
         <v>80.771799999999999</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1070,7 +1070,7 @@
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1090,7 +1090,7 @@
         <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1127,7 +1127,7 @@
         <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1198,7 +1198,7 @@
         <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1235,7 +1235,7 @@
         <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1255,7 +1255,7 @@
         <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>75</v>
       </c>
       <c r="F31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1329,7 +1329,7 @@
         <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
         <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.4">
@@ -1386,7 +1386,7 @@
         <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
adding 5 new members and modified the excel file
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Lasith sir\Alumni Locator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lasith sir\Alumni-Locator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980DEBF-37FA-435E-9206-08A537D2D899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1286CD-FDE4-43FB-8262-569020BCD857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17880" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="152">
   <si>
     <t>Name on Screen</t>
   </si>
@@ -444,13 +444,61 @@
   </si>
   <si>
     <t>immgs/shashiki.jpg</t>
+  </si>
+  <si>
+    <t>Ganguli</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>https://lk.linkedin.com/in/ganguli-ranasinghe</t>
+  </si>
+  <si>
+    <t>immgs/ganguli.jpg</t>
+  </si>
+  <si>
+    <t>Dilani</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dilanisajeewani/</t>
+  </si>
+  <si>
+    <t>immgs/Dilani.jpg</t>
+  </si>
+  <si>
+    <t>Lakshani</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ashara-athukorala-927398249/</t>
+  </si>
+  <si>
+    <t>Lakshani .jpg</t>
+  </si>
+  <si>
+    <t>Nirosha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/niroshakj/</t>
+  </si>
+  <si>
+    <t>Nirosha .jpg</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chathuri-wijesekara/</t>
+  </si>
+  <si>
+    <t>Chathuri.jpg</t>
+  </si>
+  <si>
+    <t>Chathuri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,13 +520,46 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -494,10 +575,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -779,13 +867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.21875" customWidth="1"/>
@@ -794,7 +882,7 @@
     <col min="6" max="6" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +902,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="24">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -834,7 +922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="24">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -854,7 +942,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="24">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -874,7 +962,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="24">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -894,7 +982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="24">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -914,7 +1002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -934,7 +1022,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="24">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -954,7 +1042,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -974,7 +1062,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="24">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -994,7 +1082,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="24">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1102,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="24">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1034,7 +1122,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="24">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1054,7 +1142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="24">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1074,7 +1162,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="24">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1094,7 +1182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="24">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1114,7 +1202,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="24">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1122,10 +1210,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>7.8731</v>
+        <v>37.813600000000001</v>
       </c>
       <c r="D17" s="2">
-        <v>80.771799999999999</v>
+        <v>144.9631</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>96</v>
@@ -1134,7 +1222,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="24">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1154,7 +1242,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="24">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1174,7 +1262,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="24">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1194,7 +1282,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="24">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1214,7 +1302,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="24">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1234,7 +1322,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="24">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1254,7 +1342,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="24">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1274,7 +1362,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="24">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1294,7 +1382,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="24">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1314,7 +1402,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="24">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1334,7 +1422,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="24">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1342,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="2">
-        <v>6.7106000000000003</v>
+        <v>56.130400000000002</v>
       </c>
       <c r="D28" s="2">
-        <v>79.907399999999996</v>
+        <v>106.3468</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>70</v>
@@ -1354,7 +1442,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1374,7 +1462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="24">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1394,7 +1482,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="24">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1414,7 +1502,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="24">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1434,7 +1522,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1454,7 +1542,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="24">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1474,12 +1562,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="24">
       <c r="A35" t="s">
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C35" s="2">
         <v>43.653199999999998</v>
@@ -1494,18 +1582,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="24">
       <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C36" s="2">
-        <v>6.8018000000000001</v>
+        <v>49.282699999999998</v>
       </c>
       <c r="D36">
-        <v>79.922700000000006</v>
+        <v>123.1207</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>78</v>
@@ -1514,7 +1602,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="24">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -1534,7 +1622,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="24">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -1554,7 +1642,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="24">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -1574,7 +1662,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="24">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -1594,8 +1682,107 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="24" x14ac:dyDescent="0.4">
-      <c r="C41" s="2"/>
+    <row r="41" spans="1:7" ht="24">
+      <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="2">
+        <v>26.066700000000001</v>
+      </c>
+      <c r="D41">
+        <v>50.557699999999997</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="24">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="2">
+        <v>33.8688</v>
+      </c>
+      <c r="D42">
+        <v>151.20930000000001</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="4">
+        <v>25.2744</v>
+      </c>
+      <c r="D43" s="4">
+        <v>133.77510000000001</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4">
+        <v>42.040900000000001</v>
+      </c>
+      <c r="D44" s="4">
+        <v>146.80869999999999</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" ht="24">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="2">
+        <v>7.2906000000000004</v>
+      </c>
+      <c r="D45">
+        <v>80.633700000000005</v>
+      </c>
+      <c r="E45" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1634,8 +1821,12 @@
     <hyperlink ref="E17" r:id="rId33" xr:uid="{0603ACEF-9B14-4402-ACC8-D9D5BBA66E69}"/>
     <hyperlink ref="E37" r:id="rId34" xr:uid="{4B8E632E-55DD-4057-B12E-31A441D04F47}"/>
     <hyperlink ref="E38" r:id="rId35" xr:uid="{8D7BFB67-CCA1-4727-B1AE-53D90AA100B3}"/>
+    <hyperlink ref="E41" r:id="rId36" xr:uid="{6EA6D80E-DB21-439D-9FD3-68B5E5B04B4E}"/>
+    <hyperlink ref="E42" r:id="rId37" xr:uid="{CDAD1D80-F047-49B9-875B-C4FB3FB39726}"/>
+    <hyperlink ref="E43" r:id="rId38" xr:uid="{84E60EEE-F6AD-47BA-BD4F-56252C308B2F}"/>
+    <hyperlink ref="E44" r:id="rId39" xr:uid="{75B37D7D-450C-4590-845A-FA9B4482DBD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding new members and files'
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lasith sir\Alumni-Locator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA82F1C1-5F70-4AB3-9A79-813C2D8D14F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC48973-0CB4-4C6F-BC93-F4D44ABE2B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
   <si>
     <t>Name on Screen</t>
   </si>
@@ -492,6 +492,33 @@
   </si>
   <si>
     <t>immgs/Chathuri.jpg</t>
+  </si>
+  <si>
+    <t>Chamith</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chamith-nadeeshan/</t>
+  </si>
+  <si>
+    <t>Chamith.jpg</t>
+  </si>
+  <si>
+    <t>Hansani</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hansani-gunathilaka/</t>
+  </si>
+  <si>
+    <t>Hansani .jpg</t>
+  </si>
+  <si>
+    <t>Gayashan</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/pasindu-gayashan/</t>
+  </si>
+  <si>
+    <t>Gayashan.jpg</t>
   </si>
 </sst>
 </file>
@@ -867,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1210,10 +1237,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>37.813600000000001</v>
+        <v>-23.2744</v>
       </c>
       <c r="D17" s="2">
-        <v>144.9631</v>
+        <v>133.77510000000001</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>96</v>
@@ -1710,7 +1737,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="2">
-        <v>-33.8688</v>
+        <v>-21.8688</v>
       </c>
       <c r="D42">
         <v>151.20930000000001</v>
@@ -1783,6 +1810,69 @@
       <c r="F45" t="s">
         <v>151</v>
       </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="4">
+        <v>6.9271000000000003</v>
+      </c>
+      <c r="D46" s="4">
+        <v>79.861199999999997</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="4">
+        <v>6.9271000000000003</v>
+      </c>
+      <c r="D47" s="4">
+        <v>79.861199999999997</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="4">
+        <v>6.9271000000000003</v>
+      </c>
+      <c r="D48" s="4">
+        <v>79.861199999999997</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1825,8 +1915,11 @@
     <hyperlink ref="E42" r:id="rId37" xr:uid="{CDAD1D80-F047-49B9-875B-C4FB3FB39726}"/>
     <hyperlink ref="E43" r:id="rId38" xr:uid="{84E60EEE-F6AD-47BA-BD4F-56252C308B2F}"/>
     <hyperlink ref="E44" r:id="rId39" xr:uid="{75B37D7D-450C-4590-845A-FA9B4482DBD9}"/>
+    <hyperlink ref="E46" r:id="rId40" xr:uid="{F199FFFA-4AC5-46DA-986B-0BC058C9E2DC}"/>
+    <hyperlink ref="E47" r:id="rId41" xr:uid="{B8A4B9CC-498B-4A75-A76D-B9AE1246D2EA}"/>
+    <hyperlink ref="E48" r:id="rId42" xr:uid="{1E6809BC-CD4F-4CE9-A681-6EF3A40FE249}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
back to previous file
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lasith sir\Alumni-Locator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23418B5C-85DF-494A-AB5E-B24751FD5883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013A70D1-6B71-4671-83B2-483D703C069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="206">
   <si>
     <t>Name on Screen</t>
   </si>
@@ -519,13 +519,148 @@
   </si>
   <si>
     <t>immgs/Gayashan.jpg</t>
+  </si>
+  <si>
+    <t>Thilini</t>
+  </si>
+  <si>
+    <t>https://lk.linkedin.com/in/thilini-rambukwella</t>
+  </si>
+  <si>
+    <t>Zikra</t>
+  </si>
+  <si>
+    <t>https://lk.linkedin.com/in/zikrafazil</t>
+  </si>
+  <si>
+    <t>Hansini</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hansini-abesinghe-/</t>
+  </si>
+  <si>
+    <t>Achini</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/achini-hanchapola-bb39251aa/</t>
+  </si>
+  <si>
+    <t>Tharanga</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/tharangapathirana/</t>
+  </si>
+  <si>
+    <t>Nipuni</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nipuni-fernando-83b23619b/</t>
+  </si>
+  <si>
+    <t>Judith</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/judith-harriet-francke/</t>
+  </si>
+  <si>
+    <t>Ayomi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ayomi-sandarekha/</t>
+  </si>
+  <si>
+    <t>Kasun</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kasun-pradeep-wanshapala-8b8311206/</t>
+  </si>
+  <si>
+    <t>Uditha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/uditha-sampath/</t>
+  </si>
+  <si>
+    <t>Sandaru</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sandarumalshan/</t>
+  </si>
+  <si>
+    <t>Sadeepa</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sadeepa-rukshan/</t>
+  </si>
+  <si>
+    <t>Prathibha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/prathibha-warnasinghe-17424719b/</t>
+  </si>
+  <si>
+    <t>Randi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/randi-jayawardhana-43056319b/</t>
+  </si>
+  <si>
+    <t>Thisari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/thisari-gunasekara-0aab681b6/</t>
+  </si>
+  <si>
+    <t>immgs/thilini.jpg</t>
+  </si>
+  <si>
+    <t>immgs/zikra.jpg</t>
+  </si>
+  <si>
+    <t>immgs/hansini.jpg</t>
+  </si>
+  <si>
+    <t>immgs/achini.jpg</t>
+  </si>
+  <si>
+    <t>immgs/tharanga.jpg</t>
+  </si>
+  <si>
+    <t>immgs/nipuni.jpg</t>
+  </si>
+  <si>
+    <t>immgs/judith.jpg</t>
+  </si>
+  <si>
+    <t>immgs/ayomi.jpg</t>
+  </si>
+  <si>
+    <t>immgs/kasunw.jpg</t>
+  </si>
+  <si>
+    <t>immgs/uditha.jpg</t>
+  </si>
+  <si>
+    <t>immgs/Sandaru.jpg</t>
+  </si>
+  <si>
+    <t>immgs/sadeepa.jpg</t>
+  </si>
+  <si>
+    <t>immgs/prathibha.jpg</t>
+  </si>
+  <si>
+    <t>immgs/randi.jpg</t>
+  </si>
+  <si>
+    <t>immgs/thisari.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,6 +709,17 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FFE8EAED"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -602,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -613,6 +759,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -894,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1873,6 +2022,306 @@
         <v>160</v>
       </c>
       <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" ht="24">
+      <c r="A49" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="9">
+        <v>7.2906000000000004</v>
+      </c>
+      <c r="D49" s="8">
+        <v>80.633700000000005</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="4">
+        <v>6.9271000000000003</v>
+      </c>
+      <c r="D50" s="4">
+        <v>70.861199999999997</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="4">
+        <v>7.4675000000000002</v>
+      </c>
+      <c r="D51" s="4">
+        <v>82.623400000000004</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="4">
+        <v>7.0839999999999996</v>
+      </c>
+      <c r="D52" s="4">
+        <v>84.009799999999998</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="4">
+        <v>7.0839999999999996</v>
+      </c>
+      <c r="D53" s="4">
+        <v>88.009799999999998</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="4">
+        <v>6.9271000000000003</v>
+      </c>
+      <c r="D54" s="4">
+        <v>79.861199999999997</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="4">
+        <v>6.8270999999999997</v>
+      </c>
+      <c r="D55" s="4">
+        <v>79.861199999999997</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="4">
+        <v>6.7956000000000003</v>
+      </c>
+      <c r="D56" s="4">
+        <v>81.236400000000003</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="4">
+        <v>6.6271000000000004</v>
+      </c>
+      <c r="D57" s="4">
+        <v>72.861199999999997</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="4">
+        <v>6.5270999999999999</v>
+      </c>
+      <c r="D58" s="4">
+        <v>77.861199999999997</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="4">
+        <v>6.8270999999999997</v>
+      </c>
+      <c r="D59" s="4">
+        <v>75.861199999999997</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="4">
+        <v>6.6271000000000004</v>
+      </c>
+      <c r="D60" s="4">
+        <v>77.861199999999997</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="4">
+        <v>6.4271000000000003</v>
+      </c>
+      <c r="D61" s="4">
+        <v>76.861199999999997</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="4">
+        <v>6.8270999999999997</v>
+      </c>
+      <c r="D62" s="4">
+        <v>77.861199999999997</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="4">
+        <v>6.4271000000000003</v>
+      </c>
+      <c r="D63" s="4">
+        <v>78.861199999999997</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1918,8 +2367,23 @@
     <hyperlink ref="E46" r:id="rId40" xr:uid="{F199FFFA-4AC5-46DA-986B-0BC058C9E2DC}"/>
     <hyperlink ref="E47" r:id="rId41" xr:uid="{B8A4B9CC-498B-4A75-A76D-B9AE1246D2EA}"/>
     <hyperlink ref="E48" r:id="rId42" xr:uid="{1E6809BC-CD4F-4CE9-A681-6EF3A40FE249}"/>
+    <hyperlink ref="E49" r:id="rId43" xr:uid="{94A5641F-9DAD-4D95-AF99-D40583F94177}"/>
+    <hyperlink ref="E50" r:id="rId44" xr:uid="{34DAD309-AC42-47BF-8F65-51246FD3CA57}"/>
+    <hyperlink ref="E51" r:id="rId45" xr:uid="{746D27AF-DC9E-4F5E-9A8C-A66D0D3D371D}"/>
+    <hyperlink ref="E52" r:id="rId46" xr:uid="{136259D9-9404-47BD-B4F5-B009A5BC0089}"/>
+    <hyperlink ref="E53" r:id="rId47" xr:uid="{E92E862D-C32E-4C24-A827-6F8C94151103}"/>
+    <hyperlink ref="E54" r:id="rId48" xr:uid="{FD680E4E-5329-43C4-86CB-844C36CAA06E}"/>
+    <hyperlink ref="E55" r:id="rId49" xr:uid="{DD3B34AA-E931-4BF2-B4AF-4E5CDFDD37A8}"/>
+    <hyperlink ref="E56" r:id="rId50" xr:uid="{2B4CBC4A-B7D4-4BE7-8AD4-25760D16E136}"/>
+    <hyperlink ref="E57" r:id="rId51" xr:uid="{31E87A03-AFDD-402D-8E19-EB2194717B8B}"/>
+    <hyperlink ref="E58" r:id="rId52" xr:uid="{065CCA77-EE36-45AE-90C8-97D8FBCFB53F}"/>
+    <hyperlink ref="E59" r:id="rId53" xr:uid="{936E0DA3-3101-4CBB-9AB5-FD3560C9DC07}"/>
+    <hyperlink ref="E60" r:id="rId54" xr:uid="{54A7603C-7D90-4448-90E6-B9CFD04CE1D5}"/>
+    <hyperlink ref="E61" r:id="rId55" xr:uid="{8175245D-7233-4ACB-9E01-7B3A6E71B6B9}"/>
+    <hyperlink ref="E62" r:id="rId56" xr:uid="{B0E5DBDA-BD83-4D0F-B857-0FCA8461D439}"/>
+    <hyperlink ref="E63" r:id="rId57" xr:uid="{8692D5FC-7168-4413-A251-070CDDC91A2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>